<commit_message>
feat -> implement class for excel
</commit_message>
<xml_diff>
--- a/maktabkhooneh_98521081.xlsx
+++ b/maktabkhooneh_98521081.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="maktabkhoone_course_list" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
   <si>
     <t>عنوان دوره</t>
   </si>
@@ -50,6 +50,384 @@
   </si>
   <si>
     <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%A7%D9%82%D8%AA%D8%B5%D8%A7%D8%AF-%D9%85%D9%87%D9%86%D8%AF%D8%B3%DB%8C-mk1364/</t>
+  </si>
+  <si>
+    <t>آموزش مدیریت سرور و امنیت در لینوکس | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Greg Williams</t>
+  </si>
+  <si>
+    <t>مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>49,000</t>
+  </si>
+  <si>
+    <t>3 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D9%85%D8%AF%DB%8C%D8%B1%DB%8C%D8%AA-%D8%B3%D8%B1%D9%88%D8%B1-%D8%A7%D9%85%D9%86%DB%8C%D8%AA-%D9%84%DB%8C%D9%86%D9%88%DA%A9%D8%B3-mk1330/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان آمار و احتمال | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>28 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%A2%D9%85%D8%A7%D8%B1-%D8%A7%D8%AD%D8%AA%D9%85%D8%A7%D9%84-mk1365/</t>
+  </si>
+  <si>
+    <t>آموزش گوگل آنالیتیکس برای مبتدیان - مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Justin Cutroni</t>
+  </si>
+  <si>
+    <t>Krista Seiden</t>
+  </si>
+  <si>
+    <t>29,000</t>
+  </si>
+  <si>
+    <t>1:03 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%DA%AF%D9%88%DA%AF%D9%84-%D8%A2%D9%86%D8%A7%D9%84%DB%8C%D8%AA%DB%8C%DA%A9%D8%B3-%D9%85%D8%A8%D8%AA%D8%AF%DB%8C%D8%A7%D9%86-mk1325/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان پایتون کاربردی | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>سروش حیدری پهلویان</t>
+  </si>
+  <si>
+    <t>9 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D9%BE%D8%A7%DB%8C%D8%AA%D9%88%D9%86-%DA%A9%D8%A7%D8%B1%D8%A8%D8%B1%D8%AF%DB%8C-mk1352/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان یادگیری عمیق با پایتون | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>7 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%DB%8C%D8%A7%D8%AF%DA%AF%DB%8C%D8%B1%DB%8C-%D8%B9%D9%85%DB%8C%D9%82-%D8%A8%D8%A7-%D9%BE%D8%A7%DB%8C%D8%AA%D9%88%D9%86-mk1353/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان فلاتر برای همه | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>امیر احمد ادیبی</t>
+  </si>
+  <si>
+    <t>5 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D9%81%D9%84%D8%A7%D8%AA%D8%B1-%D8%A8%D8%B1%D8%A7%DB%8C-%D9%87%D9%85%D9%87-mk1329/</t>
+  </si>
+  <si>
+    <t>آموزش ASP.NET Core برای ورود به بازار کار | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>رامین محمدحسینی</t>
+  </si>
+  <si>
+    <t>249,000</t>
+  </si>
+  <si>
+    <t>32 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-asp-net-core-mk1290/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان دینامیک سازه‌ها | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>رضا رؤفی</t>
+  </si>
+  <si>
+    <t>دانشگاه آزاد اسلامی واحد اهواز</t>
+  </si>
+  <si>
+    <t>16 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%AF%DB%8C%D9%86%D8%A7%D9%85%DB%8C%DA%A9-%D8%B3%D8%A7%D8%B2%D9%87%D9%87%D8%A7-mk1302/</t>
+  </si>
+  <si>
+    <t>آموزش کارگردانی با فرزاد مؤتمن | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>فرزاد مؤتمن</t>
+  </si>
+  <si>
+    <t>299,000</t>
+  </si>
+  <si>
+    <t>14 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%DA%A9%D8%A7%D8%B1%DA%AF%D8%B1%D8%AF%D8%A7%D9%86%DB%8C-%D9%81%D8%B1%D8%B2%D8%A7%D8%AF-%D9%85%D9%88%D8%AA%D9%85%D9%86-mk1355/</t>
+  </si>
+  <si>
+    <t>آموزش مرحله اول المپیاد ریاضی (رایگان) | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>سپهر عسگری</t>
+  </si>
+  <si>
+    <t>11 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D9%85%D8%B1%D8%AD%D9%84%D9%87-%D8%A7%D9%88%D9%84-%D8%A7%D9%84%D9%85%D9%BE%DB%8C%D8%A7%D8%AF-%D8%B1%DB%8C%D8%A7%D8%B6%DB%8C-mk1354/</t>
+  </si>
+  <si>
+    <t>آموزش ساخت فروشگاه اینترنتی با چند فروشنده | آموزش وردپرس | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Nayyar Shaikh</t>
+  </si>
+  <si>
+    <t>Udemy</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%A7%D9%81%D8%B2%D9%88%D9%86%D9%87-%DA%86%D9%86%D8%AF-%D9%81%D8%B1%D9%88%D8%B4%D9%86%D8%AF%DA%AF%DB%8C-%D9%88%D9%88%DA%A9%D8%A7%D9%85%D8%B1%D8%B3-%D8%AF%DA%A9%D8%A7%D9%86-mk1340/</t>
+  </si>
+  <si>
+    <t>پردازش موازی در پایتون | آموزش پردازش موازی | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>محمدرضا کریمی‌نژاد</t>
+  </si>
+  <si>
+    <t>39,000</t>
+  </si>
+  <si>
+    <t>5 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D9%BE%D8%B1%D8%AF%D8%A7%D8%B2%D8%B4-%D9%85%D9%88%D8%A7%D8%B2%DB%8C-%D9%BE%D8%A7%DB%8C%D8%AA%D9%88%D9%86-mk1346/</t>
+  </si>
+  <si>
+    <t>آموزش جامع طراحی و تحلیل الگوریتم‌ها | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>محمد گنج‌تابش</t>
+  </si>
+  <si>
+    <t>15 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%AC%D8%A7%D9%85%D8%B9-%D8%B7%D8%B1%D8%A7%D8%AD%DB%8C-%D8%A7%D9%84%DA%AF%D9%88%D8%B1%DB%8C%D8%AA%D9%85-mk1351/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان C# | آموزش برنامه نویسی سی شارپ رایگان | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>امیررضا تابش‌فرد</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%B3%DB%8C-%D8%B4%D8%A7%D8%B1%D9%BE-mk1312/</t>
+  </si>
+  <si>
+    <t>آموزش رایتینگ آیلتس تسک 2 | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>شان محمدی</t>
+  </si>
+  <si>
+    <t>8 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%D8%AA%DB%8C%D9%86%DA%AF-%D8%A2%DB%8C%D9%84%D8%AA%D8%B3-mk1343/</t>
+  </si>
+  <si>
+    <t>آموزش لیسنینگ آیلتس | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>7 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D9%84%DB%8C%D8%B3%D9%86%DB%8C%D9%86%DA%AF-%D8%A7%DB%8C%D9%84%D8%AA%D8%B3-mk1344/</t>
+  </si>
+  <si>
+    <t>آموزش ریدینگ آیلتس | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%DB%8C%D8%AF%DB%8C%D9%86%DA%AF-%D8%A2%DB%8C%D9%84%D8%AA%D8%B3-mk1349/</t>
+  </si>
+  <si>
+    <t>آموزش تحلیل بازارهای مالی با مفهوم بنگاه‌داری بانک‌ ها  | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>عباس دادجوی توکلی</t>
+  </si>
+  <si>
+    <t>احسان راکعی</t>
+  </si>
+  <si>
+    <t>79,000</t>
+  </si>
+  <si>
+    <t>2 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A8%D9%86%DA%AF%D8%A7%D9%87-%D8%AF%D8%A7%D8%B1%DB%8C-%D8%A8%D8%A7%D9%86%DA%A9-%D9%87%D8%A7-mk1345/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان دینامیک | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>علي محمد شافعی</t>
+  </si>
+  <si>
+    <t>دانشگاه شهید باهنر کرمان</t>
+  </si>
+  <si>
+    <t>30 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%AF%DB%8C%D9%86%D8%A7%D9%85%DB%8C%DA%A9-mk1341/</t>
+  </si>
+  <si>
+    <t>آموزش جامع تحقیقات بازار | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>مجید عقلایی</t>
+  </si>
+  <si>
+    <t>649,000</t>
+  </si>
+  <si>
+    <t>55 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%AA%D8%AD%D9%82%DB%8C%D9%82%D8%A7%D8%AA-%D8%A8%D8%A7%D8%B2%D8%A7%D8%B1-mk1248/</t>
+  </si>
+  <si>
+    <t>گریم سینمایی | آموزش گریم سینمایی | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>امیر ترابی</t>
+  </si>
+  <si>
+    <t>179,000</t>
+  </si>
+  <si>
+    <t>6 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%DA%AF%D8%B1%DB%8C%D9%85-%D8%B3%DB%8C%D9%86%D9%85%D8%A7%DB%8C%DB%8C-mk1336/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان روش‌های تولید | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>علیرضا صادقی</t>
+  </si>
+  <si>
+    <t>31 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%B1%D9%88%D8%B4-%D8%AA%D9%88%D9%84%DB%8C%D8%AF-mk1338/</t>
+  </si>
+  <si>
+    <t>آموزش نقد فیلم با مسعود فراستی | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>مسعود فراستی</t>
+  </si>
+  <si>
+    <t>169,000</t>
+  </si>
+  <si>
+    <t>9 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D9%86%D9%82%D8%AF-%D9%81%DB%8C%D9%84%D9%85-mk1335/</t>
+  </si>
+  <si>
+    <t>آموزش شطرنج با گری کاسپاروف | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Garry Kasparov</t>
+  </si>
+  <si>
+    <t>Master Class</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B4%D8%B7%D8%B1%D9%86%D8%AC-%DA%AF%D8%B1%DB%8C-%DA%A9%D8%A7%D8%B3%D9%BE%D8%A7%D8%B1%D9%88%D9%81-mk1291/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان مبانی برنامه‌نویسی | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>محمد امین فضلی</t>
+  </si>
+  <si>
+    <t>دانشگاه صنعتی شریف</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D9%85%D8%A8%D8%A7%D9%86%DB%8C-%D8%A8%D8%B1%D9%86%D8%A7%D9%85%D9%87-%D9%86%D9%88%DB%8C%D8%B3%DB%8C-mk1342/</t>
+  </si>
+  <si>
+    <t>آموزش رایگان تحلیل ماتریسی سازه‌ها | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>مهدی شاداب‌فر</t>
+  </si>
+  <si>
+    <t>3 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%AA%D8%AD%D9%84%DB%8C%D9%84-%D9%85%D8%A7%D8%AA%D8%B1%DB%8C%D8%B3-%D8%B3%D8%A7%D8%B2%D9%87-mk1337/</t>
+  </si>
+  <si>
+    <t>بازی‌سازی با اسکرچ | برنامه‌نویسی اسکرچ | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Al Sweigart</t>
+  </si>
+  <si>
+    <t>139,000</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A8%D8%A7%D8%B2%DB%8C-%D8%B3%D8%A7%D8%B2%DB%8C-%D8%A8%D8%A7-%D8%A7%D8%B3%DA%A9%D8%B1%DA%86-mk1321/</t>
+  </si>
+  <si>
+    <t>مهارت‌های اکسل برای کسب و کار | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Nicky Bull</t>
+  </si>
+  <si>
+    <t>Prashan Karunaratne</t>
+  </si>
+  <si>
+    <t>4 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D9%85%D9%87%D8%A7%D8%B1%D8%AA-%D9%87%D8%A7%DB%8C-%D8%A7%DA%A9%D8%B3%D9%84-%D8%A8%D8%B1%D8%A7%DB%8C-%DA%A9%D8%B3%D8%A8-%D9%88-%DA%A9%D8%A7%D8%B1-mk1307/</t>
+  </si>
+  <si>
+    <t>گوگل ادز | آموزش گوگل ads، ادوردز | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Jesper Sohlin</t>
+  </si>
+  <si>
+    <t>Robin Nordin</t>
+  </si>
+  <si>
+    <t>16 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%DA%AF%D9%88%DA%AF%D9%84-%D8%A7%D8%AF%D8%B2-mk1293/</t>
   </si>
 </sst>
 </file>
@@ -394,7 +772,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,9 +818,618 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F17" r:id="rId16"/>
+    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F19" r:id="rId18"/>
+    <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F21" r:id="rId20"/>
+    <hyperlink ref="F22" r:id="rId21"/>
+    <hyperlink ref="F23" r:id="rId22"/>
+    <hyperlink ref="F24" r:id="rId23"/>
+    <hyperlink ref="F25" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId25"/>
+    <hyperlink ref="F27" r:id="rId26"/>
+    <hyperlink ref="F28" r:id="rId27"/>
+    <hyperlink ref="F29" r:id="rId28"/>
+    <hyperlink ref="F30" r:id="rId29"/>
+    <hyperlink ref="F31" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat -> implement environment class
</commit_message>
<xml_diff>
--- a/maktabkhooneh_98521081.xlsx
+++ b/maktabkhooneh_98521081.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>عنوان دوره</t>
   </si>
@@ -32,19 +32,62 @@
   </si>
   <si>
     <t>لینک</t>
+  </si>
+  <si>
+    <t>آموزش رایگان اقتصاد مهندسی | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>نوید خادمی</t>
+  </si>
+  <si>
+    <t>دانشگاه تهران</t>
+  </si>
+  <si>
+    <t>رایگان</t>
+  </si>
+  <si>
+    <t>14 جلسه</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.orghttps://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D8%B1%D8%A7%DB%8C%DA%AF%D8%A7%D9%86-%D8%A7%D9%82%D8%AA%D8%B5%D8%A7%D8%AF-%D9%85%D9%87%D9%86%D8%AF%D8%B3%DB%8C-mk1364/</t>
+  </si>
+  <si>
+    <t>آموزش مدیریت سرور و امنیت در لینوکس | مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>Greg Williams</t>
+  </si>
+  <si>
+    <t>مکتب‌خونه</t>
+  </si>
+  <si>
+    <t>49,000</t>
+  </si>
+  <si>
+    <t>3 ساعت</t>
+  </si>
+  <si>
+    <t>https://maktabkhooneh.orghttps://maktabkhooneh.org/course/%D8%A2%D9%85%D9%88%D8%B2%D8%B4-%D9%85%D8%AF%DB%8C%D8%B1%DB%8C%D8%AA-%D8%B3%D8%B1%D9%88%D8%B1-%D8%A7%D9%85%D9%86%DB%8C%D8%AA-%D9%84%DB%8C%D9%86%D9%88%DA%A9%D8%B3-mk1330/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,13 +107,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,7 +438,51 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>